<commit_message>
tablas de importacion de novedades
</commit_message>
<xml_diff>
--- a/20181115 - Cronograma personalizaciones ERP - CCG.xlsx
+++ b/20181115 - Cronograma personalizaciones ERP - CCG.xlsx
@@ -832,7 +832,7 @@
   <dimension ref="A1:W68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2045,7 +2045,7 @@
       <c r="D34" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E34" s="30" t="s">
         <v>44</v>
       </c>
       <c r="F34" s="2"/>
@@ -2080,7 +2080,7 @@
       <c r="D35" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="E35" s="30" t="s">
         <v>44</v>
       </c>
       <c r="F35" s="2"/>
@@ -2115,7 +2115,7 @@
       <c r="D36" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="E36" s="30" t="s">
         <v>44</v>
       </c>
       <c r="F36" s="2"/>

</xml_diff>

<commit_message>
Update 20181115 - Cronograma personalizaciones ERP - CCG.xlsx
</commit_message>
<xml_diff>
--- a/20181115 - Cronograma personalizaciones ERP - CCG.xlsx
+++ b/20181115 - Cronograma personalizaciones ERP - CCG.xlsx
@@ -828,11 +828,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:W68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -894,84 +893,84 @@
       </c>
       <c r="E2" s="4">
         <f ca="1">TODAY()+4</f>
-        <v>43429</v>
+        <v>43430</v>
       </c>
       <c r="F2" s="4">
         <f ca="1">E2+1</f>
-        <v>43430</v>
+        <v>43431</v>
       </c>
       <c r="G2" s="5">
         <f t="shared" ref="G2:W2" ca="1" si="0">F2+1</f>
-        <v>43431</v>
+        <v>43432</v>
       </c>
       <c r="H2" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>43432</v>
+        <v>43433</v>
       </c>
       <c r="I2" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>43433</v>
+        <v>43434</v>
       </c>
       <c r="J2" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>43434</v>
+        <v>43435</v>
       </c>
       <c r="K2" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>43435</v>
+        <v>43436</v>
       </c>
       <c r="L2" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>43436</v>
+        <v>43437</v>
       </c>
       <c r="M2" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>43437</v>
+        <v>43438</v>
       </c>
       <c r="N2" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>43438</v>
+        <v>43439</v>
       </c>
       <c r="O2" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>43439</v>
+        <v>43440</v>
       </c>
       <c r="P2" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>43440</v>
+        <v>43441</v>
       </c>
       <c r="Q2" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>43441</v>
+        <v>43442</v>
       </c>
       <c r="R2" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>43442</v>
+        <v>43443</v>
       </c>
       <c r="S2" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>43443</v>
+        <v>43444</v>
       </c>
       <c r="T2" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>43444</v>
+        <v>43445</v>
       </c>
       <c r="U2" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>43445</v>
+        <v>43446</v>
       </c>
       <c r="V2" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>43446</v>
+        <v>43447</v>
       </c>
       <c r="W2" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>43447</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+        <v>43448</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>
@@ -1210,7 +1209,7 @@
       <c r="V9" s="2"/>
       <c r="W9" s="2"/>
     </row>
-    <row r="10" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -1245,7 +1244,7 @@
       <c r="V10" s="2"/>
       <c r="W10" s="2"/>
     </row>
-    <row r="11" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -1348,7 +1347,7 @@
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
     </row>
-    <row r="14" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -1383,7 +1382,7 @@
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
     </row>
-    <row r="15" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -1453,7 +1452,7 @@
       <c r="V16" s="2"/>
       <c r="W16" s="2"/>
     </row>
-    <row r="17" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
@@ -1587,7 +1586,7 @@
       <c r="V20" s="2"/>
       <c r="W20" s="2"/>
     </row>
-    <row r="21" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>29</v>
       </c>
@@ -1657,7 +1656,7 @@
       <c r="V22" s="2"/>
       <c r="W22" s="2"/>
     </row>
-    <row r="23" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>29</v>
       </c>
@@ -1692,7 +1691,7 @@
       <c r="V23" s="2"/>
       <c r="W23" s="2"/>
     </row>
-    <row r="24" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
@@ -1760,7 +1759,7 @@
       <c r="V25" s="2"/>
       <c r="W25" s="2"/>
     </row>
-    <row r="26" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
@@ -1863,7 +1862,7 @@
       <c r="V28" s="2"/>
       <c r="W28" s="2"/>
     </row>
-    <row r="29" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>42</v>
       </c>
@@ -1964,7 +1963,7 @@
       <c r="V31" s="2"/>
       <c r="W31" s="2"/>
     </row>
-    <row r="32" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A32" s="13" t="s">
         <v>48</v>
       </c>
@@ -2067,7 +2066,7 @@
       <c r="V34" s="2"/>
       <c r="W34" s="2"/>
     </row>
-    <row r="35" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>48</v>
       </c>
@@ -2102,7 +2101,7 @@
       <c r="V35" s="2"/>
       <c r="W35" s="2"/>
     </row>
-    <row r="36" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>48</v>
       </c>
@@ -2205,7 +2204,7 @@
       <c r="V38" s="2"/>
       <c r="W38" s="2"/>
     </row>
-    <row r="39" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A39" s="18" t="s">
         <v>48</v>
       </c>
@@ -2271,7 +2270,7 @@
       <c r="V40" s="2"/>
       <c r="W40" s="2"/>
     </row>
-    <row r="41" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>48</v>
       </c>
@@ -2306,7 +2305,7 @@
       <c r="V41" s="2"/>
       <c r="W41" s="2"/>
     </row>
-    <row r="42" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A42" s="13" t="s">
         <v>48</v>
       </c>
@@ -2339,7 +2338,7 @@
       <c r="V42" s="2"/>
       <c r="W42" s="2"/>
     </row>
-    <row r="43" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>48</v>
       </c>
@@ -2374,7 +2373,7 @@
       <c r="V43" s="2"/>
       <c r="W43" s="2"/>
     </row>
-    <row r="44" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>61</v>
       </c>
@@ -2409,7 +2408,7 @@
       <c r="V44" s="2"/>
       <c r="W44" s="2"/>
     </row>
-    <row r="45" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>61</v>
       </c>
@@ -2444,7 +2443,7 @@
       <c r="V45" s="2"/>
       <c r="W45" s="2"/>
     </row>
-    <row r="46" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A46" s="13" t="s">
         <v>64</v>
       </c>
@@ -2477,7 +2476,7 @@
       <c r="V46" s="2"/>
       <c r="W46" s="2"/>
     </row>
-    <row r="47" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A47" s="20" t="s">
         <v>64</v>
       </c>
@@ -2720,7 +2719,7 @@
       <c r="V53" s="2"/>
       <c r="W53" s="2"/>
     </row>
-    <row r="54" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>48</v>
       </c>
@@ -2757,7 +2756,7 @@
       <c r="V54" s="2"/>
       <c r="W54" s="2"/>
     </row>
-    <row r="55" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>48</v>
       </c>
@@ -2792,7 +2791,7 @@
       <c r="V55" s="2"/>
       <c r="W55" s="2"/>
     </row>
-    <row r="56" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>48</v>
       </c>
@@ -2827,7 +2826,7 @@
       <c r="V56" s="2"/>
       <c r="W56" s="2"/>
     </row>
-    <row r="57" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>48</v>
       </c>
@@ -2862,7 +2861,7 @@
       <c r="V57" s="2"/>
       <c r="W57" s="2"/>
     </row>
-    <row r="58" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>48</v>
       </c>
@@ -2897,7 +2896,7 @@
       <c r="V58" s="2"/>
       <c r="W58" s="2"/>
     </row>
-    <row r="59" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>48</v>
       </c>
@@ -2932,7 +2931,7 @@
       <c r="V59" s="2"/>
       <c r="W59" s="2"/>
     </row>
-    <row r="60" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>48</v>
       </c>
@@ -2965,7 +2964,7 @@
       <c r="V60" s="2"/>
       <c r="W60" s="2"/>
     </row>
-    <row r="61" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>48</v>
       </c>
@@ -3000,7 +2999,7 @@
       <c r="V61" s="2"/>
       <c r="W61" s="2"/>
     </row>
-    <row r="62" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>48</v>
       </c>
@@ -3035,7 +3034,7 @@
       <c r="V62" s="2"/>
       <c r="W62" s="2"/>
     </row>
-    <row r="63" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>48</v>
       </c>
@@ -3070,7 +3069,7 @@
       <c r="V63" s="2"/>
       <c r="W63" s="2"/>
     </row>
-    <row r="64" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>48</v>
       </c>
@@ -3125,7 +3124,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>86</v>
       </c>
@@ -3158,7 +3157,7 @@
       <c r="V65" s="2"/>
       <c r="W65" s="2"/>
     </row>
-    <row r="66" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>88</v>
       </c>
@@ -3197,7 +3196,7 @@
       <c r="V66" s="2"/>
       <c r="W66" s="2"/>
     </row>
-    <row r="67" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>88</v>
       </c>
@@ -3236,7 +3235,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="68" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>88</v>
       </c>
@@ -3276,13 +3275,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:W68">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="IOBANDO"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A2:W68"/>
   <mergeCells count="3">
     <mergeCell ref="E1:J1"/>
     <mergeCell ref="L1:Q1"/>

</xml_diff>